<commit_message>
Arreglamos las columnas cedula y comentarios. Columna otrosPagos agregada
</commit_message>
<xml_diff>
--- a/assets/data/ExcelToJson.NominaOnly.xlsx
+++ b/assets/data/ExcelToJson.NominaOnly.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luizestevo/Documents/projects/js/Nomina/assets/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ariel\OneDrive\Documents\Proyectos\serSalud.Nomina\Nomina\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93BDD21-8026-7346-994D-44C854097292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="540" windowWidth="26340" windowHeight="14340" xr2:uid="{F9448C94-4D34-184E-B2D5-08575244DE69}"/>
+    <workbookView xWindow="675" yWindow="540" windowWidth="26340" windowHeight="14340"/>
   </bookViews>
   <sheets>
     <sheet name="Nomina" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="72">
   <si>
     <t>ESTRELLITA DOMINICANA MEJIA GIL</t>
   </si>
@@ -114,9 +113,6 @@
     <t>SI</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>LICENCIA MEDICA</t>
   </si>
   <si>
@@ -252,25 +248,16 @@
     <t>otrosPagos</t>
   </si>
   <si>
-    <t>facturcion</t>
-  </si>
-  <si>
-    <t>notasDeFacturacion</t>
-  </si>
-  <si>
-    <t>nombreDelSolicitante</t>
-  </si>
-  <si>
-    <t>cargoDelSolicitante</t>
-  </si>
-  <si>
-    <t>TelefonoDelSolicitate</t>
+    <t>08:05AM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-10409]hh:mm\ AM/PM;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -280,7 +267,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,6 +277,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,8 +316,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,98 +633,78 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B2C7CF-6969-1140-AFF7-A5E1B13A8C3C}">
-  <dimension ref="A1:T17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A17"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="97.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -742,13 +717,16 @@
       <c r="E2" t="s">
         <v>21</v>
       </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
       <c r="G2" t="s">
         <v>22</v>
       </c>
-      <c r="H2">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="I2">
+      <c r="H2" s="2">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="I2" s="2">
         <v>0.95833333333333337</v>
       </c>
       <c r="J2" t="s">
@@ -761,25 +739,10 @@
         <v>25</v>
       </c>
       <c r="N2" t="s">
-        <v>71</v>
-      </c>
-      <c r="P2" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>73</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>20</v>
       </c>
@@ -790,22 +753,22 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
         <v>27</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
       </c>
       <c r="G3" t="s">
         <v>0</v>
       </c>
-      <c r="H3">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="I3">
+      <c r="H3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="2">
         <v>0.83333333333333337</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K3" t="s">
         <v>24</v>
@@ -813,15 +776,8 @@
       <c r="L3" t="s">
         <v>25</v>
       </c>
-      <c r="R3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T3" s="1"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>20</v>
       </c>
@@ -832,22 +788,22 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
         <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>
       </c>
-      <c r="H4">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="I4">
+      <c r="H4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="2">
         <v>0.75</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K4" t="s">
         <v>24</v>
@@ -855,15 +811,8 @@
       <c r="L4" t="s">
         <v>25</v>
       </c>
-      <c r="R4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T4" s="1"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -874,41 +823,34 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="J5" t="s">
         <v>32</v>
-      </c>
-      <c r="H5">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="I5">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="J5" t="s">
-        <v>33</v>
       </c>
       <c r="K5" t="s">
         <v>24</v>
       </c>
       <c r="L5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" t="s">
         <v>34</v>
       </c>
-      <c r="O5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T5" s="1"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>20</v>
       </c>
@@ -922,16 +864,16 @@
         <v>21</v>
       </c>
       <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="J6" t="s">
         <v>36</v>
-      </c>
-      <c r="H6">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I6">
-        <v>0.27777777777777779</v>
-      </c>
-      <c r="J6" t="s">
-        <v>37</v>
       </c>
       <c r="K6" t="s">
         <v>24</v>
@@ -940,17 +882,10 @@
         <v>1000</v>
       </c>
       <c r="O6" t="s">
-        <v>38</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T6" s="1"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>20</v>
       </c>
@@ -964,16 +899,16 @@
         <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I7">
+        <v>35</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="2">
         <v>0.27777777777777779</v>
       </c>
       <c r="J7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K7" t="s">
         <v>24</v>
@@ -982,17 +917,10 @@
         <v>1000</v>
       </c>
       <c r="O7" t="s">
-        <v>40</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T7" s="1"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>20</v>
       </c>
@@ -1006,16 +934,16 @@
         <v>21</v>
       </c>
       <c r="F8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="J8" t="s">
         <v>41</v>
-      </c>
-      <c r="H8">
-        <v>0.25</v>
-      </c>
-      <c r="I8">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="J8" t="s">
-        <v>42</v>
       </c>
       <c r="K8" t="s">
         <v>24</v>
@@ -1023,15 +951,8 @@
       <c r="M8">
         <v>900</v>
       </c>
-      <c r="R8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T8" s="1"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>20</v>
       </c>
@@ -1042,22 +963,22 @@
         <v>16</v>
       </c>
       <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
         <v>43</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>44</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="J9" t="s">
         <v>45</v>
-      </c>
-      <c r="H9">
-        <v>0.375</v>
-      </c>
-      <c r="I9">
-        <v>0.625</v>
-      </c>
-      <c r="J9" t="s">
-        <v>46</v>
       </c>
       <c r="K9" t="s">
         <v>24</v>
@@ -1065,15 +986,8 @@
       <c r="L9" t="s">
         <v>25</v>
       </c>
-      <c r="R9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T9" s="1"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>20</v>
       </c>
@@ -1084,22 +998,22 @@
         <v>16</v>
       </c>
       <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
         <v>43</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>44</v>
       </c>
-      <c r="G10" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10">
-        <v>0.375</v>
-      </c>
-      <c r="I10">
+      <c r="H10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="J10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K10" t="s">
         <v>24</v>
@@ -1107,15 +1021,8 @@
       <c r="L10" t="s">
         <v>25</v>
       </c>
-      <c r="R10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T10" s="1"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>20</v>
       </c>
@@ -1126,32 +1033,25 @@
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11">
-        <v>0.375</v>
-      </c>
-      <c r="I11">
+        <v>43</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="J11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K11" t="s">
         <v>24</v>
       </c>
-      <c r="R11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T11" s="1"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>20</v>
       </c>
@@ -1162,19 +1062,19 @@
         <v>10</v>
       </c>
       <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
         <v>48</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="J12" t="s">
         <v>49</v>
-      </c>
-      <c r="H12">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="I12">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="J12" t="s">
-        <v>50</v>
       </c>
       <c r="K12" t="s">
         <v>24</v>
@@ -1182,15 +1082,8 @@
       <c r="L12" t="s">
         <v>25</v>
       </c>
-      <c r="R12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T12" s="1"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>20</v>
       </c>
@@ -1201,22 +1094,22 @@
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G13" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="J13" t="s">
         <v>51</v>
-      </c>
-      <c r="H13">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="I13">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="J13" t="s">
-        <v>52</v>
       </c>
       <c r="K13" t="s">
         <v>24</v>
@@ -1224,15 +1117,8 @@
       <c r="L13" t="s">
         <v>25</v>
       </c>
-      <c r="R13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T13" s="1"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>20</v>
       </c>
@@ -1243,22 +1129,22 @@
         <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" t="s">
         <v>53</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="J14" t="s">
         <v>54</v>
-      </c>
-      <c r="H14">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="I14">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="J14" t="s">
-        <v>55</v>
       </c>
       <c r="K14" t="s">
         <v>24</v>
@@ -1266,14 +1152,8 @@
       <c r="L14" t="s">
         <v>25</v>
       </c>
-      <c r="R14" t="s">
-        <v>26</v>
-      </c>
-      <c r="S14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>20</v>
       </c>
@@ -1284,40 +1164,34 @@
         <v>6</v>
       </c>
       <c r="E15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" t="s">
         <v>27</v>
-      </c>
-      <c r="F15" t="s">
-        <v>28</v>
       </c>
       <c r="G15" t="s">
         <v>0</v>
       </c>
-      <c r="H15">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="I15">
+      <c r="H15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I15" s="2">
         <v>0.75</v>
       </c>
       <c r="J15" t="s">
+        <v>55</v>
+      </c>
+      <c r="K15" t="s">
         <v>56</v>
-      </c>
-      <c r="K15" t="s">
-        <v>57</v>
       </c>
       <c r="L15" t="s">
         <v>25</v>
       </c>
       <c r="O15" t="s">
-        <v>58</v>
-      </c>
-      <c r="R15" t="s">
-        <v>26</v>
-      </c>
-      <c r="S15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>20</v>
       </c>
@@ -1328,40 +1202,34 @@
         <v>6</v>
       </c>
       <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" t="s">
         <v>27</v>
-      </c>
-      <c r="F16" t="s">
-        <v>28</v>
       </c>
       <c r="G16" t="s">
         <v>0</v>
       </c>
-      <c r="H16">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="I16">
+      <c r="H16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" s="2">
         <v>0.83333333333333337</v>
       </c>
       <c r="J16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L16" t="s">
         <v>25</v>
       </c>
       <c r="O16" t="s">
-        <v>58</v>
-      </c>
-      <c r="R16" t="s">
-        <v>26</v>
-      </c>
-      <c r="S16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>20</v>
       </c>
@@ -1375,26 +1243,24 @@
         <v>21</v>
       </c>
       <c r="F17" t="s">
-        <v>28</v>
-      </c>
-      <c r="H17">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I17">
+        <v>27</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I17" s="2">
         <v>0.27777777777777779</v>
       </c>
       <c r="J17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K17" t="s">
-        <v>57</v>
-      </c>
-      <c r="R17" t="s">
-        <v>26</v>
-      </c>
-      <c r="S17" t="s">
-        <v>26</v>
-      </c>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tabla actualizada al español
</commit_message>
<xml_diff>
--- a/assets/data/ExcelToJson.NominaOnly.xlsx
+++ b/assets/data/ExcelToJson.NominaOnly.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="71">
   <si>
     <t>ESTRELLITA DOMINICANA MEJIA GIL</t>
   </si>
@@ -246,9 +246,6 @@
   </si>
   <si>
     <t>otrosPagos</t>
-  </si>
-  <si>
-    <t>08:05AM</t>
   </si>
 </sst>
 </file>
@@ -636,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -724,7 +721,7 @@
         <v>22</v>
       </c>
       <c r="H2" s="2">
-        <v>0.33680555555555558</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="I2" s="2">
         <v>0.95833333333333337</v>
@@ -761,8 +758,8 @@
       <c r="G3" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>71</v>
+      <c r="H3" s="2">
+        <v>0.33333333333333331</v>
       </c>
       <c r="I3" s="2">
         <v>0.83333333333333337</v>
@@ -796,8 +793,8 @@
       <c r="G4" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>71</v>
+      <c r="H4" s="2">
+        <v>0.33333333333333331</v>
       </c>
       <c r="I4" s="2">
         <v>0.75</v>
@@ -831,8 +828,8 @@
       <c r="G5" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>71</v>
+      <c r="H5" s="2">
+        <v>0.58333333333333337</v>
       </c>
       <c r="I5" s="2">
         <v>0.83333333333333337</v>
@@ -866,8 +863,8 @@
       <c r="F6" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>71</v>
+      <c r="H6" s="2">
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="I6" s="2">
         <v>0.27777777777777779</v>
@@ -901,8 +898,8 @@
       <c r="F7" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>71</v>
+      <c r="H7" s="2">
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="I7" s="2">
         <v>0.27777777777777779</v>
@@ -936,8 +933,8 @@
       <c r="F8" t="s">
         <v>40</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>71</v>
+      <c r="H8" s="2">
+        <v>0.25</v>
       </c>
       <c r="I8" s="2">
         <v>0.45833333333333331</v>
@@ -971,8 +968,8 @@
       <c r="G9" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>71</v>
+      <c r="H9" s="2">
+        <v>0.375</v>
       </c>
       <c r="I9" s="2">
         <v>0.625</v>
@@ -1006,8 +1003,8 @@
       <c r="G10" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>71</v>
+      <c r="H10" s="2">
+        <v>0.375</v>
       </c>
       <c r="I10" s="2">
         <v>0.54166666666666663</v>
@@ -1038,8 +1035,8 @@
       <c r="F11" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>71</v>
+      <c r="H11" s="2">
+        <v>0.375</v>
       </c>
       <c r="I11" s="2">
         <v>0.54166666666666663</v>
@@ -1067,8 +1064,8 @@
       <c r="F12" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>71</v>
+      <c r="H12" s="2">
+        <v>0.29166666666666669</v>
       </c>
       <c r="I12" s="2">
         <v>0.79166666666666663</v>
@@ -1102,8 +1099,8 @@
       <c r="G13" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>71</v>
+      <c r="H13" s="2">
+        <v>0.29166666666666669</v>
       </c>
       <c r="I13" s="2">
         <v>0.79166666666666663</v>
@@ -1137,8 +1134,8 @@
       <c r="G14" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>71</v>
+      <c r="H14" s="2">
+        <v>0.79166666666666663</v>
       </c>
       <c r="I14" s="2">
         <v>0.29166666666666669</v>
@@ -1172,8 +1169,8 @@
       <c r="G15" t="s">
         <v>0</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>71</v>
+      <c r="H15" s="2">
+        <v>0.33333333333333331</v>
       </c>
       <c r="I15" s="2">
         <v>0.75</v>
@@ -1210,8 +1207,8 @@
       <c r="G16" t="s">
         <v>0</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>71</v>
+      <c r="H16" s="2">
+        <v>0.33333333333333331</v>
       </c>
       <c r="I16" s="2">
         <v>0.83333333333333337</v>
@@ -1245,8 +1242,8 @@
       <c r="F17" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>71</v>
+      <c r="H17" s="2">
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="I17" s="2">
         <v>0.27777777777777779</v>

</xml_diff>